<commit_message>
Add support for population range matrices. First step towards addressing issue 133.
</commit_message>
<xml_diff>
--- a/pacehrh/tests/simple_config/super_simple_inputs.xlsx
+++ b/pacehrh/tests/simple_config/super_simple_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlesel\Source\Ethiopia-HEP-Capacity-Analysis\pacehrh\tests\simple_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66FD35B-2776-42DF-B317-3B42739E7F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4BE423-A4B9-44E8-88E6-F91305A4DF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="1005" windowWidth="21600" windowHeight="9465" tabRatio="830" firstSheet="1" activeTab="3" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="5340" yWindow="0" windowWidth="21600" windowHeight="10200" tabRatio="830" activeTab="6" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="80" r:id="rId1"/>
@@ -18,37 +18,51 @@
     <sheet name="Flat_Rates" sheetId="90" r:id="rId3"/>
     <sheet name="Rise_Rates" sheetId="93" r:id="rId4"/>
     <sheet name="Flat_StochasticParms" sheetId="91" r:id="rId5"/>
-    <sheet name="TEST_StochasticParms" sheetId="76" r:id="rId6"/>
-    <sheet name="TEST_TotalPop" sheetId="74" r:id="rId7"/>
-    <sheet name="TEST_PopValues" sheetId="75" r:id="rId8"/>
-    <sheet name="TEST_PopValues_Const" sheetId="77" r:id="rId9"/>
-    <sheet name="TEST_TaskValues" sheetId="78" r:id="rId10"/>
-    <sheet name="TEST_TaskValues_1" sheetId="81" r:id="rId11"/>
-    <sheet name="EXP_PopValues" sheetId="84" r:id="rId12"/>
-    <sheet name="newPopValues" sheetId="88" r:id="rId13"/>
-    <sheet name="TEST_SeasonalityCurves_1" sheetId="82" r:id="rId14"/>
-    <sheet name="PopValues" sheetId="56" r:id="rId15"/>
-    <sheet name="TaskValues" sheetId="57" r:id="rId16"/>
-    <sheet name="StochasticParameters" sheetId="72" r:id="rId17"/>
-    <sheet name="SeasonalityCurves" sheetId="58" r:id="rId18"/>
-    <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId19"/>
+    <sheet name="Lookup" sheetId="94" r:id="rId6"/>
+    <sheet name="Bad_Lookup" sheetId="95" r:id="rId7"/>
+    <sheet name="TEST_StochasticParms" sheetId="76" r:id="rId8"/>
+    <sheet name="TEST_TotalPop" sheetId="74" r:id="rId9"/>
+    <sheet name="TEST_PopValues_Const" sheetId="77" r:id="rId10"/>
+    <sheet name="TEST_TaskValues" sheetId="78" r:id="rId11"/>
+    <sheet name="TEST_TaskValues_1" sheetId="81" r:id="rId12"/>
+    <sheet name="EXP_PopValues" sheetId="84" r:id="rId13"/>
+    <sheet name="newPopValues" sheetId="88" r:id="rId14"/>
+    <sheet name="TEST_SeasonalityCurves_1" sheetId="82" r:id="rId15"/>
+    <sheet name="PopValues" sheetId="56" r:id="rId16"/>
+    <sheet name="TaskValues" sheetId="57" r:id="rId17"/>
+    <sheet name="StochasticParameters" sheetId="72" r:id="rId18"/>
+    <sheet name="SeasonalityCurves" sheetId="58" r:id="rId19"/>
+    <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId20"/>
     <externalReference r:id="rId21"/>
     <externalReference r:id="rId22"/>
+    <externalReference r:id="rId23"/>
+    <externalReference r:id="rId24"/>
+    <externalReference r:id="rId25"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">TaskValues!$A$1:$S$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">TaskValues!$A$1:$S$103</definedName>
+    <definedName name="hours" localSheetId="6">#REF!</definedName>
+    <definedName name="hours" localSheetId="5">#REF!</definedName>
     <definedName name="hours" localSheetId="0">#REF!</definedName>
     <definedName name="hours">#REF!</definedName>
+    <definedName name="select_pop" localSheetId="6">#REF!</definedName>
+    <definedName name="select_pop" localSheetId="5">#REF!</definedName>
     <definedName name="select_pop" localSheetId="0">#REF!</definedName>
     <definedName name="select_pop">#REF!</definedName>
-    <definedName name="total_pop" localSheetId="0">[1]Demographics_Total!$CZ$3</definedName>
+    <definedName name="select_pop_2">'[1]Inputs Assump'!$C$4</definedName>
+    <definedName name="total_pop" localSheetId="6">[2]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop" localSheetId="5">[2]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop" localSheetId="0">[2]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop">#REF!</definedName>
-    <definedName name="total_pop_2">[1]Demographics_Total!$CZ$3</definedName>
-    <definedName name="total_pop2" localSheetId="0">[2]Demographics_Total!$CZ$3</definedName>
-    <definedName name="total_pop2">[3]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop_2">[2]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2" localSheetId="6">[3]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2" localSheetId="5">[3]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2" localSheetId="0">[4]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2">[5]Demographics_Total!$CZ$3</definedName>
+    <definedName name="weeks" localSheetId="6">#REF!</definedName>
+    <definedName name="weeks" localSheetId="5">#REF!</definedName>
     <definedName name="weeks" localSheetId="0">#REF!</definedName>
     <definedName name="weeks">#REF!</definedName>
   </definedNames>
@@ -71,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="427">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1307,6 +1321,51 @@
   </si>
   <si>
     <t>MortalityM</t>
+  </si>
+  <si>
+    <t>Clinical Category</t>
+  </si>
+  <si>
+    <t>Service Category</t>
+  </si>
+  <si>
+    <t>Relevant Population Labels</t>
+  </si>
+  <si>
+    <t>Starting Age</t>
+  </si>
+  <si>
+    <t>Ending Age</t>
+  </si>
+  <si>
+    <t>Preventive</t>
+  </si>
+  <si>
+    <t>Chronic</t>
+  </si>
+  <si>
+    <t>Sexual health</t>
+  </si>
+  <si>
+    <t>Acute</t>
+  </si>
+  <si>
+    <t>NTDs</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>0-100</t>
+  </si>
+  <si>
+    <t>35-55</t>
+  </si>
+  <si>
+    <t>xxx_Female</t>
+  </si>
+  <si>
+    <t>yyy_Male</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1384,7 @@
     <numFmt numFmtId="171" formatCode="0.00000000"/>
     <numFmt numFmtId="172" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1404,6 +1463,21 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1495,7 +1569,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1550,6 +1624,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1582,6 +1658,141 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="TEST_TotalPop"/>
+      <sheetName val="TEST_PopValues_Const"/>
+      <sheetName val="TEST_StochasticParms"/>
+      <sheetName val="TEST_TaskValues"/>
+      <sheetName val="TEST_TaskValues_1"/>
+      <sheetName val="TEST_PopValues"/>
+      <sheetName val="To Do or Upgrade"/>
+      <sheetName val="TEST_SeasonalityCurves_1"/>
+      <sheetName val="Scenarios"/>
+      <sheetName val="Data dictionary Scenarios"/>
+      <sheetName val="TotalPop"/>
+      <sheetName val="Lookup"/>
+      <sheetName val="PopValues"/>
+      <sheetName val="TaskValues"/>
+      <sheetName val="StochasticParamaters"/>
+      <sheetName val="AgeSpecific Fertility"/>
+      <sheetName val="RuralUrban Mortality"/>
+      <sheetName val="Fertility mod check"/>
+      <sheetName val="Ratios"/>
+      <sheetName val="SeasonalityCurves"/>
+      <sheetName val="SeasonalityOffsets"/>
+      <sheetName val="Services summary"/>
+      <sheetName val="AggregateDALYs"/>
+      <sheetName val="Prevalences"/>
+      <sheetName val="DALYs "/>
+      <sheetName val="CEA"/>
+      <sheetName val="Work time"/>
+      <sheetName val="Ssn TB"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Ssn Malaria"/>
+      <sheetName val="Ssn Nutr"/>
+      <sheetName val="Ssn Measles"/>
+      <sheetName val="Sheet21"/>
+      <sheetName val="Services ref"/>
+      <sheetName val="Coverage impacts"/>
+      <sheetName val="Inputs Assump"/>
+      <sheetName val="Demographics_Total"/>
+      <sheetName val="Pop M"/>
+      <sheetName val="Pop F"/>
+      <sheetName val="TB Incidence"/>
+      <sheetName val="Malaria Incid"/>
+      <sheetName val="FP mod"/>
+      <sheetName val="unmet need"/>
+      <sheetName val="HIV Prev"/>
+      <sheetName val="HIV Incid"/>
+      <sheetName val="fertility"/>
+      <sheetName val="fertility 15-19"/>
+      <sheetName val="mort infant"/>
+      <sheetName val="mort 1-5"/>
+      <sheetName val="mort 5-9"/>
+      <sheetName val="mort 10-14"/>
+      <sheetName val="mort 15-19"/>
+      <sheetName val="mort 20-24"/>
+      <sheetName val="mort adult f"/>
+      <sheetName val="mort adult m"/>
+      <sheetName val="Staffing Ratios"/>
+      <sheetName val="Demographics_InCalc"/>
+      <sheetName val="Births"/>
+      <sheetName val="Mortality"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35">
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Total national</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1646,81 +1857,95 @@
       <sheetName val="mort adult f"/>
       <sheetName val="mort adult m"/>
       <sheetName val="AggregateDALYs"/>
+      <sheetName val="PopValues_retain"/>
+      <sheetName val="NCD age group"/>
+      <sheetName val="Fertility Mortality Rates"/>
+      <sheetName val="Lookup"/>
+      <sheetName val="PopRegional2020"/>
+      <sheetName val="Pop_female_2020"/>
+      <sheetName val="Pop_male_2020"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
       <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
       <sheetData sheetId="43">
         <row r="3">
           <cell r="CZ3">
-            <v>115103531.71799999</v>
+            <v>24715222.24724872</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1863,7 +2088,150 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="To Do or Upgrade"/>
+      <sheetName val="Inputs Assump"/>
+      <sheetName val="C FTE Equiv"/>
+      <sheetName val="C Tot Hrs by Cat"/>
+      <sheetName val="C Variance"/>
+      <sheetName val="Time Summary"/>
+      <sheetName val="C Hrs by Category (3)"/>
+      <sheetName val="C Hrs by Category (2)"/>
+      <sheetName val="C Ratio to Baseline"/>
+      <sheetName val="Pie 2020"/>
+      <sheetName val="Calculations"/>
+      <sheetName val="Demographics_InCalc"/>
+      <sheetName val="Births"/>
+      <sheetName val="Mortality"/>
+      <sheetName val="FH.MC"/>
+      <sheetName val="FH.FP"/>
+      <sheetName val="FH.Im"/>
+      <sheetName val="FH.N"/>
+      <sheetName val="DPC"/>
+      <sheetName val="Other"/>
+      <sheetName val="DATA"/>
+      <sheetName val="Ssn Malaria"/>
+      <sheetName val="Ssn Nutr"/>
+      <sheetName val="Ssn Measles"/>
+      <sheetName val="Demographics_Total"/>
+      <sheetName val="Prevalences"/>
+      <sheetName val="Work time"/>
+      <sheetName val="Sheet21"/>
+      <sheetName val="Services summary"/>
+      <sheetName val="Services ref"/>
+      <sheetName val="Coverage impacts"/>
+      <sheetName val="Pop M"/>
+      <sheetName val="Pop F"/>
+      <sheetName val="TB Incidence"/>
+      <sheetName val="Malaria Incid"/>
+      <sheetName val="C Fertility"/>
+      <sheetName val="fertility"/>
+      <sheetName val="FP mod"/>
+      <sheetName val="unmet need"/>
+      <sheetName val="HIV Prev"/>
+      <sheetName val="HIV Incid"/>
+      <sheetName val="mort infant"/>
+      <sheetName val="mort 1-5"/>
+      <sheetName val="mort 5-9"/>
+      <sheetName val="mort 10-14"/>
+      <sheetName val="mort 15-19"/>
+      <sheetName val="mort 20-24"/>
+      <sheetName val="mort adult f"/>
+      <sheetName val="mort adult m"/>
+      <sheetName val="Staffing Ratios"/>
+      <sheetName val="fertility 15-19"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Ratio max rural</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11">
+        <row r="4">
+          <cell r="V4">
+            <v>105.34416988791497</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24">
+        <row r="3">
+          <cell r="CZ3">
+            <v>115103531.71799999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39">
+        <row r="77">
+          <cell r="BC77">
+            <v>1.4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="40">
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>Ethiopia</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2585,6 +2953,359 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995A7145-A7A2-400E-A46D-7F405050A633}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>4.0484955677198515</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.12294985225732839</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6">
+        <v>0.19850000000000001</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7">
+        <v>0.14050000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8">
+        <v>3.15E-2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>44.870649522800001</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>3.5500000000000007</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>1.1800000000000002</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>0.96</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>1.6</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14">
+        <v>1.72</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>3.9443060860274208</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>5.1027857526880149</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B18">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23">
+        <v>4.6410387643786963</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>289</v>
+      </c>
+      <c r="B24">
+        <v>7.8897658994437831</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B25">
+        <v>22.091344518442593</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26">
+        <v>243.00478970286852</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>292</v>
+      </c>
+      <c r="B27">
+        <v>6.3527026636382198</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>293</v>
+      </c>
+      <c r="B28">
+        <v>12.070135060912618</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29">
+        <v>31.382351158372806</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>295</v>
+      </c>
+      <c r="B30">
+        <v>273.02645507784337</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2EFC64-DD10-4E27-BDEE-F8164111A157}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -6999,7 +7720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC92EF8-ED58-4F68-8888-9CEAC4C59B7E}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -7179,7 +7900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E7F677-BE8D-4B15-BFBB-F131739569D4}">
   <sheetPr>
     <tabColor theme="1"/>
@@ -8073,7 +8794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4F2564-875C-4CBF-A10D-C89D0A9C38FE}">
   <sheetPr>
     <tabColor theme="1"/>
@@ -8967,7 +9688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C257F5-E6CC-4BAC-9A98-0BD35FA17AEF}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -9388,7 +10109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B914963F-A73F-44CC-BA92-87184BB1A8C7}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -9834,7 +10555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D83D06-B7B0-4361-896A-BFF57EC1D426}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -14831,7 +15552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDCD1CB-9612-4FAF-ACD4-A7C81D8F794C}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -14957,7 +15678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1975A502-7E7F-4553-BC06-71CD8A16214F}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -15315,396 +16036,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FB9B18-434F-4677-A182-407CBC10EA8F}">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:I22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H1" t="s">
-        <v>282</v>
-      </c>
-      <c r="I1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <v>-7</v>
-      </c>
-      <c r="E2">
-        <v>-5</v>
-      </c>
-      <c r="F2">
-        <v>-3</v>
-      </c>
-      <c r="G2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C8" t="s">
-        <v>200</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C11" t="s">
-        <v>200</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1">
-        <v>12</v>
-      </c>
-      <c r="H11" s="1">
-        <v>14</v>
-      </c>
-      <c r="I11" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B13" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>213</v>
-      </c>
-      <c r="B14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>249</v>
-      </c>
-      <c r="B15" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>251</v>
-      </c>
-      <c r="B16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>253</v>
-      </c>
-      <c r="B17" t="s">
-        <v>215</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>250</v>
-      </c>
-      <c r="B18" t="s">
-        <v>215</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>252</v>
-      </c>
-      <c r="B19" t="s">
-        <v>215</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" t="s">
-        <v>216</v>
-      </c>
-      <c r="C20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" t="s">
-        <v>180</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -17251,6 +17582,396 @@
       <c r="D102">
         <f t="shared" si="1"/>
         <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FB9B18-434F-4677-A182-407CBC10EA8F}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>-7</v>
+      </c>
+      <c r="E2">
+        <v>-5</v>
+      </c>
+      <c r="F2">
+        <v>-3</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -17489,7 +18210,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -17833,6 +18554,1032 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DA224C-9F4E-4904-8642-99CF70167D50}">
+  <dimension ref="B1:J142"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>413</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>35</v>
+      </c>
+      <c r="J4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111"/>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F112"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F115"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F116"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F117"/>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F118"/>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F119"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F120"/>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F121"/>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F122"/>
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F123"/>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F124"/>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F125"/>
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F126"/>
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F127"/>
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F128"/>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F129"/>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F130"/>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F131"/>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F132"/>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F133"/>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F134"/>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F135"/>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F136"/>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F137"/>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F138"/>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F139"/>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F140"/>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F141"/>
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F142"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA08B31E-403F-4D98-A2C5-BD7B3834450E}">
+  <dimension ref="B1:J142"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>413</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>35</v>
+      </c>
+      <c r="J4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111"/>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F112"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F115"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F116"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F117"/>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F118"/>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F119"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F120"/>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F121"/>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F122"/>
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F123"/>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F124"/>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F125"/>
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F126"/>
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F127"/>
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F128"/>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F129"/>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F130"/>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F131"/>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F132"/>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F133"/>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F134"/>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F135"/>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F136"/>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F137"/>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F138"/>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F139"/>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F140"/>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F141"/>
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F142"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9D8C93-D1F0-4C18-9265-2678791347D8}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -17958,7 +19705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1C1D20-CB4E-4F81-BAF5-8FCEF2CFF00C}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -19506,710 +21253,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512EFF05-775C-43A2-9B3E-1FF481FEDDFB}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:C30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>4.0484955677198515</v>
-      </c>
-      <c r="C2">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>0.12294985225732839</v>
-      </c>
-      <c r="C4">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="C5">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B6">
-        <v>0.19850000000000001</v>
-      </c>
-      <c r="C6">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>285</v>
-      </c>
-      <c r="B7">
-        <v>0.14050000000000001</v>
-      </c>
-      <c r="C7">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B8">
-        <v>3.15E-2</v>
-      </c>
-      <c r="C8">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <v>44.870649522800001</v>
-      </c>
-      <c r="C9">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10">
-        <v>3.5500000000000007</v>
-      </c>
-      <c r="C10">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11">
-        <v>1.1800000000000002</v>
-      </c>
-      <c r="C11">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12">
-        <v>0.96</v>
-      </c>
-      <c r="C12">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13">
-        <v>1.6</v>
-      </c>
-      <c r="C13">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>287</v>
-      </c>
-      <c r="B14">
-        <v>1.72</v>
-      </c>
-      <c r="C14">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15">
-        <v>3.9443060860274208</v>
-      </c>
-      <c r="C15">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16">
-        <v>5.1027857526880149</v>
-      </c>
-      <c r="C16">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="C17">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>234</v>
-      </c>
-      <c r="B18">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="C18">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>236</v>
-      </c>
-      <c r="B19">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="C19">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="C20">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="C21">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C22">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>288</v>
-      </c>
-      <c r="B23">
-        <v>4.6410387643786963</v>
-      </c>
-      <c r="C23">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>289</v>
-      </c>
-      <c r="B24">
-        <v>7.8897658994437831</v>
-      </c>
-      <c r="C24">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>290</v>
-      </c>
-      <c r="B25">
-        <v>22.091344518442593</v>
-      </c>
-      <c r="C25">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>291</v>
-      </c>
-      <c r="B26">
-        <v>243.00478970286852</v>
-      </c>
-      <c r="C26">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>292</v>
-      </c>
-      <c r="B27">
-        <v>6.3527026636382198</v>
-      </c>
-      <c r="C27">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>293</v>
-      </c>
-      <c r="B28">
-        <v>12.070135060912618</v>
-      </c>
-      <c r="C28">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>294</v>
-      </c>
-      <c r="B29">
-        <v>31.382351158372806</v>
-      </c>
-      <c r="C29">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>295</v>
-      </c>
-      <c r="B30">
-        <v>273.02645507784337</v>
-      </c>
-      <c r="C30">
-        <v>0.98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995A7145-A7A2-400E-A46D-7F405050A633}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:C30"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>4.0484955677198515</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>0.12294985225732839</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B6">
-        <v>0.19850000000000001</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>285</v>
-      </c>
-      <c r="B7">
-        <v>0.14050000000000001</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B8">
-        <v>3.15E-2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <v>44.870649522800001</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10">
-        <v>3.5500000000000007</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11">
-        <v>1.1800000000000002</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12">
-        <v>0.96</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13">
-        <v>1.6</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>287</v>
-      </c>
-      <c r="B14">
-        <v>1.72</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15">
-        <v>3.9443060860274208</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16">
-        <v>5.1027857526880149</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>234</v>
-      </c>
-      <c r="B18">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>236</v>
-      </c>
-      <c r="B19">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>288</v>
-      </c>
-      <c r="B23">
-        <v>4.6410387643786963</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>289</v>
-      </c>
-      <c r="B24">
-        <v>7.8897658994437831</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>290</v>
-      </c>
-      <c r="B25">
-        <v>22.091344518442593</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>291</v>
-      </c>
-      <c r="B26">
-        <v>243.00478970286852</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>292</v>
-      </c>
-      <c r="B27">
-        <v>6.3527026636382198</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>293</v>
-      </c>
-      <c r="B28">
-        <v>12.070135060912618</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>294</v>
-      </c>
-      <c r="B29">
-        <v>31.382351158372806</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>295</v>
-      </c>
-      <c r="B30">
-        <v>273.02645507784337</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update unit tests to include tests for simple computations
</commit_message>
<xml_diff>
--- a/pacehrh/tests/simple_config/super_simple_inputs.xlsx
+++ b/pacehrh/tests/simple_config/super_simple_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlesel\Source\Ethiopia-HEP-Capacity-Analysis\pacehrh\tests\simple_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA07CE5-B0B3-4A69-AAE0-02126535EFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FF2645-B94A-49F9-B1B4-AD0B719AF528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8010" yWindow="2790" windowWidth="21600" windowHeight="11475" tabRatio="830" activeTab="8" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="5880" yWindow="2355" windowWidth="21600" windowHeight="11490" tabRatio="830" firstSheet="1" activeTab="9" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="80" r:id="rId1"/>
@@ -21,39 +21,40 @@
     <sheet name="Flat_Rates" sheetId="90" r:id="rId6"/>
     <sheet name="Rise_Rates" sheetId="93" r:id="rId7"/>
     <sheet name="Flat_StochasticParms" sheetId="91" r:id="rId8"/>
-    <sheet name="TV_Simple" sheetId="97" r:id="rId9"/>
-    <sheet name="SeasonalityCurves" sheetId="58" r:id="rId10"/>
-    <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId11"/>
-    <sheet name="Bad_Lookup" sheetId="95" r:id="rId12"/>
-    <sheet name="EXP_PopValues" sheetId="84" r:id="rId13"/>
+    <sheet name="TV_Simple_1" sheetId="97" r:id="rId9"/>
+    <sheet name="TV_Simple_Many" sheetId="98" r:id="rId10"/>
+    <sheet name="SeasonalityCurves" sheetId="58" r:id="rId11"/>
+    <sheet name="SeasonalityOffsets" sheetId="66" r:id="rId12"/>
+    <sheet name="Bad_Lookup" sheetId="95" r:id="rId13"/>
+    <sheet name="EXP_PopValues" sheetId="84" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
-    <definedName name="hours" localSheetId="11">#REF!</definedName>
+    <definedName name="hours" localSheetId="12">#REF!</definedName>
     <definedName name="hours" localSheetId="1">#REF!</definedName>
     <definedName name="hours" localSheetId="0">#REF!</definedName>
     <definedName name="hours">#REF!</definedName>
-    <definedName name="select_pop" localSheetId="11">#REF!</definedName>
+    <definedName name="select_pop" localSheetId="12">#REF!</definedName>
     <definedName name="select_pop" localSheetId="1">#REF!</definedName>
     <definedName name="select_pop" localSheetId="0">#REF!</definedName>
     <definedName name="select_pop">#REF!</definedName>
     <definedName name="select_pop_2">'[1]Inputs Assump'!$C$4</definedName>
-    <definedName name="total_pop" localSheetId="11">[2]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop" localSheetId="12">[2]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop" localSheetId="1">[2]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop" localSheetId="0">[2]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop">#REF!</definedName>
     <definedName name="total_pop_2">[2]Demographics_Total!$CZ$3</definedName>
-    <definedName name="total_pop2" localSheetId="11">[3]Demographics_Total!$CZ$3</definedName>
+    <definedName name="total_pop2" localSheetId="12">[3]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop2" localSheetId="1">[3]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop2" localSheetId="0">[4]Demographics_Total!$CZ$3</definedName>
     <definedName name="total_pop2">[5]Demographics_Total!$CZ$3</definedName>
-    <definedName name="weeks" localSheetId="11">#REF!</definedName>
+    <definedName name="weeks" localSheetId="12">#REF!</definedName>
     <definedName name="weeks" localSheetId="1">#REF!</definedName>
     <definedName name="weeks" localSheetId="0">#REF!</definedName>
     <definedName name="weeks">#REF!</definedName>
@@ -76,8 +77,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Charles Eliot (he/him/his)</author>
+  </authors>
+  <commentList>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{C7706239-CFF4-4EE4-A060-6121767F1E17}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Charles Eliot (he/him/his):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Newborns only</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="279">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -874,10 +909,46 @@
     <t>Category</t>
   </si>
   <si>
-    <t>TV_Simple</t>
-  </si>
-  <si>
     <t>Flat_Rates</t>
+  </si>
+  <si>
+    <t>Task.2</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>TV_Simple_1</t>
+  </si>
+  <si>
+    <t>TEST_Simple_2</t>
+  </si>
+  <si>
+    <t>TV_Simple_Many</t>
+  </si>
+  <si>
+    <t>Task.3</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>Task.4</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>NonClinical</t>
+  </si>
+  <si>
+    <t>Task.5</t>
+  </si>
+  <si>
+    <t>Task.6</t>
+  </si>
+  <si>
+    <t>T6</t>
   </si>
 </sst>
 </file>
@@ -887,9 +958,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,6 +1034,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1057,8 +1141,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2118,26 +2202,26 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.86328125" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="14.265625" customWidth="1"/>
-    <col min="11" max="11" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
@@ -2190,7 +2274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>262</v>
       </c>
@@ -2201,7 +2285,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="3">
-        <v>5000</v>
+        <v>-1</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>17</v>
@@ -2222,10 +2306,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L2" t="s">
         <v>265</v>
-      </c>
-      <c r="L2" t="s">
-        <v>266</v>
       </c>
       <c r="M2" t="s">
         <v>176</v>
@@ -2237,6 +2321,56 @@
         <v>182</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="3">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>270</v>
+      </c>
+      <c r="L3" t="s">
+        <v>265</v>
+      </c>
+      <c r="M3" t="s">
+        <v>176</v>
+      </c>
+      <c r="N3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O3" t="s">
+        <v>182</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2246,6 +2380,296 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E868FE-3D54-4AF5-86AB-9637B7FEC08F}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>119</v>
+      </c>
+      <c r="S1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="L4">
+        <v>0.99</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1975A502-7E7F-4553-BC06-71CD8A16214F}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -2256,13 +2680,13 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="12.73046875" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="8" customWidth="1"/>
+    <col min="2" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -2282,7 +2706,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -2304,7 +2728,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2326,7 +2750,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -2348,7 +2772,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -2370,7 +2794,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2816,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -2414,7 +2838,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -2436,7 +2860,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -2458,7 +2882,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -2480,7 +2904,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -2502,7 +2926,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -2524,7 +2948,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -2552,7 +2976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FB9B18-434F-4677-A182-407CBC10EA8F}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -2563,13 +2987,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2598,7 +3022,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2621,7 +3045,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2635,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2649,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2666,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2683,7 +3107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2697,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2720,7 +3144,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -2734,7 +3158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2751,7 +3175,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2780,7 +3204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2794,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2808,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -2825,7 +3249,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -2839,7 +3263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -2853,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -2867,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -2881,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -2895,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2909,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2923,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -2942,7 +3366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA08B31E-403F-4D98-A2C5-BD7B3834450E}">
   <dimension ref="B1:J142"/>
   <sheetViews>
@@ -2950,16 +3374,16 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.86328125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" customWidth="1"/>
-    <col min="10" max="10" width="12.73046875" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>247</v>
       </c>
@@ -2982,7 +3406,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>252</v>
       </c>
@@ -3005,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>253</v>
       </c>
@@ -3028,7 +3452,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>255</v>
       </c>
@@ -3051,7 +3475,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>60</v>
       </c>
@@ -3068,7 +3492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
@@ -3077,376 +3501,376 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H24" s="3"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H29" s="3"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F55"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F56"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F57"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F58"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F59"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F60"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F62"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F63"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F64"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F80"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F82"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F86"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F87"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F88"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F89"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F90"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F91"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F92"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F93"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F94"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F95"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F96"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F103"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F104"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F105"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F106"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F107"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F108"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F109"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F110"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F111"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F112"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F113"/>
     </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F114"/>
     </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F115"/>
     </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F116"/>
     </row>
-    <row r="117" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F117"/>
     </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F118"/>
     </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F119"/>
     </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F120"/>
     </row>
-    <row r="121" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F121"/>
     </row>
-    <row r="122" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F122"/>
     </row>
-    <row r="123" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F123"/>
     </row>
-    <row r="124" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F124"/>
     </row>
-    <row r="125" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F125"/>
     </row>
-    <row r="126" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F126"/>
     </row>
-    <row r="127" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F127"/>
     </row>
-    <row r="128" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F128"/>
     </row>
-    <row r="129" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F129"/>
     </row>
-    <row r="130" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F130"/>
     </row>
-    <row r="131" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F131"/>
     </row>
-    <row r="132" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F132"/>
     </row>
-    <row r="133" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F133"/>
     </row>
-    <row r="134" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F134"/>
     </row>
-    <row r="135" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F135"/>
     </row>
-    <row r="136" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F136"/>
     </row>
-    <row r="137" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F137"/>
     </row>
-    <row r="138" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F138"/>
     </row>
-    <row r="139" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F139"/>
     </row>
-    <row r="140" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F140"/>
     </row>
-    <row r="141" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F141"/>
     </row>
-    <row r="142" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F142"/>
     </row>
   </sheetData>
@@ -3455,7 +3879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E7F677-BE8D-4B15-BFBB-F131739569D4}">
   <sheetPr>
     <tabColor theme="1"/>
@@ -3466,19 +3890,19 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3507,7 +3931,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -3527,7 +3951,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -3550,7 +3974,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -3579,7 +4003,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3608,7 +4032,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -3637,7 +4061,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -3666,7 +4090,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -3695,7 +4119,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -3724,7 +4148,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -3753,7 +4177,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>195</v>
       </c>
@@ -3776,7 +4200,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -3802,7 +4226,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>200</v>
       </c>
@@ -3831,7 +4255,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>203</v>
       </c>
@@ -3860,7 +4284,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>206</v>
       </c>
@@ -3889,7 +4313,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>209</v>
       </c>
@@ -3918,7 +4342,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>212</v>
       </c>
@@ -3947,7 +4371,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -3976,7 +4400,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>144</v>
       </c>
@@ -4005,7 +4429,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>145</v>
       </c>
@@ -4034,7 +4458,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>146</v>
       </c>
@@ -4060,7 +4484,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>219</v>
       </c>
@@ -4086,7 +4510,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>222</v>
       </c>
@@ -4115,7 +4539,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>225</v>
       </c>
@@ -4144,7 +4568,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>228</v>
       </c>
@@ -4173,7 +4597,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -4202,7 +4626,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>234</v>
       </c>
@@ -4231,7 +4655,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -4260,7 +4684,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -4289,7 +4713,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -4318,7 +4742,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -4360,16 +4784,16 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.86328125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" customWidth="1"/>
-    <col min="10" max="10" width="12.73046875" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>247</v>
       </c>
@@ -4392,7 +4816,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>252</v>
       </c>
@@ -4415,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>253</v>
       </c>
@@ -4438,7 +4862,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>255</v>
       </c>
@@ -4461,7 +4885,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>60</v>
       </c>
@@ -4478,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
@@ -4487,376 +4911,376 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H24" s="3"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H29" s="3"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F55"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F56"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F57"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F58"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F59"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F60"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F62"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F63"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F64"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F80"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F82"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F86"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F87"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F88"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F89"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F90"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F91"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F92"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F93"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F94"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F95"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F96"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F103"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F104"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F105"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F106"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F107"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F108"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F109"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F110"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F111"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F112"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F113"/>
     </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F114"/>
     </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F115"/>
     </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F116"/>
     </row>
-    <row r="117" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F117"/>
     </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F118"/>
     </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F119"/>
     </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F120"/>
     </row>
-    <row r="121" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F121"/>
     </row>
-    <row r="122" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F122"/>
     </row>
-    <row r="123" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F123"/>
     </row>
-    <row r="124" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F124"/>
     </row>
-    <row r="125" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F125"/>
     </row>
-    <row r="126" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F126"/>
     </row>
-    <row r="127" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F127"/>
     </row>
-    <row r="128" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F128"/>
     </row>
-    <row r="129" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F129"/>
     </row>
-    <row r="130" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F130"/>
     </row>
-    <row r="131" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F131"/>
     </row>
-    <row r="132" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F132"/>
     </row>
-    <row r="133" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F133"/>
     </row>
-    <row r="134" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F134"/>
     </row>
-    <row r="135" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F135"/>
     </row>
-    <row r="136" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F136"/>
     </row>
-    <row r="137" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F137"/>
     </row>
-    <row r="138" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F138"/>
     </row>
-    <row r="139" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F139"/>
     </row>
-    <row r="140" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F140"/>
     </row>
-    <row r="141" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F141"/>
     </row>
-    <row r="142" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F142"/>
     </row>
   </sheetData>
@@ -4876,12 +5300,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="11"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -4895,7 +5319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
@@ -4910,7 +5334,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -4925,7 +5349,7 @@
         <v>19800</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -4940,7 +5364,7 @@
         <v>19600</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -4955,7 +5379,7 @@
         <v>19400</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -4970,7 +5394,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -4985,7 +5409,7 @@
         <v>19000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -5000,7 +5424,7 @@
         <v>18800</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -5015,7 +5439,7 @@
         <v>18600</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -5030,7 +5454,7 @@
         <v>18400</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -5045,7 +5469,7 @@
         <v>18200</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -5060,7 +5484,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -5075,7 +5499,7 @@
         <v>17800</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -5090,7 +5514,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -5105,7 +5529,7 @@
         <v>17400</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -5120,7 +5544,7 @@
         <v>17200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>15</v>
       </c>
@@ -5135,7 +5559,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -5150,7 +5574,7 @@
         <v>16800</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -5165,7 +5589,7 @@
         <v>16600</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -5180,7 +5604,7 @@
         <v>16400</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -5195,7 +5619,7 @@
         <v>16200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>20</v>
       </c>
@@ -5210,7 +5634,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>21</v>
       </c>
@@ -5225,7 +5649,7 @@
         <v>15800</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -5240,7 +5664,7 @@
         <v>15600</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -5255,7 +5679,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>24</v>
       </c>
@@ -5270,7 +5694,7 @@
         <v>15200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>25</v>
       </c>
@@ -5285,7 +5709,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>26</v>
       </c>
@@ -5300,7 +5724,7 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>27</v>
       </c>
@@ -5315,7 +5739,7 @@
         <v>14600</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>28</v>
       </c>
@@ -5330,7 +5754,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>29</v>
       </c>
@@ -5345,7 +5769,7 @@
         <v>14200</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -5360,7 +5784,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -5375,7 +5799,7 @@
         <v>13800</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>32</v>
       </c>
@@ -5390,7 +5814,7 @@
         <v>13600</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>33</v>
       </c>
@@ -5405,7 +5829,7 @@
         <v>13400</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>34</v>
       </c>
@@ -5420,7 +5844,7 @@
         <v>13200</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>35</v>
       </c>
@@ -5435,7 +5859,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>36</v>
       </c>
@@ -5450,7 +5874,7 @@
         <v>12800</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>37</v>
       </c>
@@ -5465,7 +5889,7 @@
         <v>12600</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>38</v>
       </c>
@@ -5480,7 +5904,7 @@
         <v>12400</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>39</v>
       </c>
@@ -5495,7 +5919,7 @@
         <v>12200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>40</v>
       </c>
@@ -5510,7 +5934,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>41</v>
       </c>
@@ -5525,7 +5949,7 @@
         <v>11800</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>42</v>
       </c>
@@ -5540,7 +5964,7 @@
         <v>11600</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>43</v>
       </c>
@@ -5555,7 +5979,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>44</v>
       </c>
@@ -5570,7 +5994,7 @@
         <v>11200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>45</v>
       </c>
@@ -5585,7 +6009,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>46</v>
       </c>
@@ -5600,7 +6024,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>47</v>
       </c>
@@ -5615,7 +6039,7 @@
         <v>10600</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>48</v>
       </c>
@@ -5630,7 +6054,7 @@
         <v>10400</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>49</v>
       </c>
@@ -5645,7 +6069,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>50</v>
       </c>
@@ -5660,7 +6084,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>51</v>
       </c>
@@ -5675,7 +6099,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>52</v>
       </c>
@@ -5690,7 +6114,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>53</v>
       </c>
@@ -5705,7 +6129,7 @@
         <v>9400</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>54</v>
       </c>
@@ -5720,7 +6144,7 @@
         <v>9200</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -5735,7 +6159,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>56</v>
       </c>
@@ -5750,7 +6174,7 @@
         <v>8800</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>57</v>
       </c>
@@ -5765,7 +6189,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>58</v>
       </c>
@@ -5780,7 +6204,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -5795,7 +6219,7 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>60</v>
       </c>
@@ -5810,7 +6234,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>61</v>
       </c>
@@ -5825,7 +6249,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -5840,7 +6264,7 @@
         <v>7600</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>63</v>
       </c>
@@ -5855,7 +6279,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>64</v>
       </c>
@@ -5870,7 +6294,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>65</v>
       </c>
@@ -5885,7 +6309,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>66</v>
       </c>
@@ -5900,7 +6324,7 @@
         <v>6800</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>67</v>
       </c>
@@ -5915,7 +6339,7 @@
         <v>6600</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>68</v>
       </c>
@@ -5930,7 +6354,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>69</v>
       </c>
@@ -5945,7 +6369,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>70</v>
       </c>
@@ -5960,7 +6384,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>71</v>
       </c>
@@ -5975,7 +6399,7 @@
         <v>5800</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>72</v>
       </c>
@@ -5990,7 +6414,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>73</v>
       </c>
@@ -6005,7 +6429,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <v>74</v>
       </c>
@@ -6020,7 +6444,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>75</v>
       </c>
@@ -6035,7 +6459,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="11">
         <v>76</v>
       </c>
@@ -6050,7 +6474,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <v>77</v>
       </c>
@@ -6065,7 +6489,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <v>78</v>
       </c>
@@ -6080,7 +6504,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <v>79</v>
       </c>
@@ -6095,7 +6519,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <v>80</v>
       </c>
@@ -6110,7 +6534,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <v>81</v>
       </c>
@@ -6125,7 +6549,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <v>82</v>
       </c>
@@ -6140,7 +6564,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <v>83</v>
       </c>
@@ -6155,7 +6579,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <v>84</v>
       </c>
@@ -6170,7 +6594,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <v>85</v>
       </c>
@@ -6185,7 +6609,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <v>86</v>
       </c>
@@ -6200,7 +6624,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <v>87</v>
       </c>
@@ -6215,7 +6639,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>88</v>
       </c>
@@ -6230,7 +6654,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>89</v>
       </c>
@@ -6245,7 +6669,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>90</v>
       </c>
@@ -6260,7 +6684,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>91</v>
       </c>
@@ -6275,7 +6699,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <v>92</v>
       </c>
@@ -6290,7 +6714,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>93</v>
       </c>
@@ -6305,7 +6729,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>94</v>
       </c>
@@ -6320,7 +6744,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <v>95</v>
       </c>
@@ -6335,7 +6759,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
         <v>96</v>
       </c>
@@ -6350,7 +6774,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <v>97</v>
       </c>
@@ -6365,7 +6789,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <v>98</v>
       </c>
@@ -6380,7 +6804,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <v>99</v>
       </c>
@@ -6395,7 +6819,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <v>100</v>
       </c>
@@ -6426,12 +6850,12 @@
       <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.59765625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -6445,7 +6869,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -6456,7 +6880,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -6464,7 +6888,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -6472,7 +6896,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -6486,7 +6910,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -6497,7 +6921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>133</v>
       </c>
@@ -6508,7 +6932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -6519,7 +6943,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -6527,7 +6951,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -6552,12 +6976,12 @@
       <selection activeCell="A17" sqref="A17:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -6571,7 +6995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
@@ -6586,7 +7010,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -6601,7 +7025,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -6616,7 +7040,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -6631,7 +7055,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -6646,7 +7070,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -6661,7 +7085,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -6676,7 +7100,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -6691,7 +7115,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -6706,7 +7130,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -6721,7 +7145,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -6736,7 +7160,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -6751,7 +7175,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -6766,7 +7190,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -6781,7 +7205,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -6796,7 +7220,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>15</v>
       </c>
@@ -6811,7 +7235,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -6826,7 +7250,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -6841,7 +7265,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -6856,7 +7280,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -6871,7 +7295,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>20</v>
       </c>
@@ -6886,7 +7310,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>21</v>
       </c>
@@ -6901,7 +7325,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -6916,7 +7340,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -6931,7 +7355,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>24</v>
       </c>
@@ -6946,7 +7370,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>25</v>
       </c>
@@ -6961,7 +7385,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>26</v>
       </c>
@@ -6976,7 +7400,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>27</v>
       </c>
@@ -6991,7 +7415,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>28</v>
       </c>
@@ -7006,7 +7430,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>29</v>
       </c>
@@ -7021,7 +7445,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -7036,7 +7460,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -7051,7 +7475,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>32</v>
       </c>
@@ -7066,7 +7490,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>33</v>
       </c>
@@ -7081,7 +7505,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>34</v>
       </c>
@@ -7096,7 +7520,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>35</v>
       </c>
@@ -7111,7 +7535,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>36</v>
       </c>
@@ -7126,7 +7550,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>37</v>
       </c>
@@ -7141,7 +7565,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>38</v>
       </c>
@@ -7156,7 +7580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>39</v>
       </c>
@@ -7171,7 +7595,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>40</v>
       </c>
@@ -7186,7 +7610,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>41</v>
       </c>
@@ -7201,7 +7625,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>42</v>
       </c>
@@ -7216,7 +7640,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>43</v>
       </c>
@@ -7231,7 +7655,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>44</v>
       </c>
@@ -7246,7 +7670,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>45</v>
       </c>
@@ -7261,7 +7685,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>46</v>
       </c>
@@ -7276,7 +7700,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>47</v>
       </c>
@@ -7291,7 +7715,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>48</v>
       </c>
@@ -7306,7 +7730,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>49</v>
       </c>
@@ -7321,7 +7745,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>50</v>
       </c>
@@ -7336,7 +7760,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>51</v>
       </c>
@@ -7351,7 +7775,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>52</v>
       </c>
@@ -7366,7 +7790,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>53</v>
       </c>
@@ -7381,7 +7805,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>54</v>
       </c>
@@ -7396,7 +7820,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -7411,7 +7835,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>56</v>
       </c>
@@ -7426,7 +7850,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>57</v>
       </c>
@@ -7441,7 +7865,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>58</v>
       </c>
@@ -7456,7 +7880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -7471,7 +7895,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>60</v>
       </c>
@@ -7486,7 +7910,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>61</v>
       </c>
@@ -7501,7 +7925,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -7516,7 +7940,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>63</v>
       </c>
@@ -7531,7 +7955,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>64</v>
       </c>
@@ -7546,7 +7970,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>65</v>
       </c>
@@ -7561,7 +7985,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>66</v>
       </c>
@@ -7576,7 +8000,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>67</v>
       </c>
@@ -7591,7 +8015,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>68</v>
       </c>
@@ -7606,7 +8030,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>69</v>
       </c>
@@ -7621,7 +8045,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>70</v>
       </c>
@@ -7636,7 +8060,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>71</v>
       </c>
@@ -7651,7 +8075,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>72</v>
       </c>
@@ -7666,7 +8090,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>73</v>
       </c>
@@ -7681,7 +8105,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <v>74</v>
       </c>
@@ -7696,7 +8120,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>75</v>
       </c>
@@ -7711,7 +8135,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="11">
         <v>76</v>
       </c>
@@ -7726,7 +8150,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <v>77</v>
       </c>
@@ -7741,7 +8165,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <v>78</v>
       </c>
@@ -7756,7 +8180,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <v>79</v>
       </c>
@@ -7771,7 +8195,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <v>80</v>
       </c>
@@ -7786,7 +8210,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <v>81</v>
       </c>
@@ -7801,7 +8225,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <v>82</v>
       </c>
@@ -7816,7 +8240,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <v>83</v>
       </c>
@@ -7831,7 +8255,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <v>84</v>
       </c>
@@ -7846,7 +8270,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <v>85</v>
       </c>
@@ -7861,7 +8285,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <v>86</v>
       </c>
@@ -7876,7 +8300,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <v>87</v>
       </c>
@@ -7891,7 +8315,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>88</v>
       </c>
@@ -7906,7 +8330,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>89</v>
       </c>
@@ -7921,7 +8345,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>90</v>
       </c>
@@ -7936,7 +8360,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>91</v>
       </c>
@@ -7951,7 +8375,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <v>92</v>
       </c>
@@ -7966,7 +8390,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>93</v>
       </c>
@@ -7981,7 +8405,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>94</v>
       </c>
@@ -7996,7 +8420,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <v>95</v>
       </c>
@@ -8011,7 +8435,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
         <v>96</v>
       </c>
@@ -8026,7 +8450,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <v>97</v>
       </c>
@@ -8041,7 +8465,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <v>98</v>
       </c>
@@ -8056,7 +8480,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <v>99</v>
       </c>
@@ -8071,7 +8495,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <v>100</v>
       </c>
@@ -8102,20 +8526,20 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -8144,7 +8568,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -8170,7 +8594,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -8196,7 +8620,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>241</v>
       </c>
@@ -8226,7 +8650,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -8252,7 +8676,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>243</v>
       </c>
@@ -8281,7 +8705,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -8326,20 +8750,20 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -8368,7 +8792,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -8394,7 +8818,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -8420,7 +8844,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>241</v>
       </c>
@@ -8450,7 +8874,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -8476,7 +8900,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>243</v>
       </c>
@@ -8505,7 +8929,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -8550,12 +8974,12 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.59765625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -8569,7 +8993,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -8580,7 +9004,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -8588,7 +9012,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -8596,7 +9020,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -8610,7 +9034,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -8621,7 +9045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>133</v>
       </c>
@@ -8632,7 +9056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -8643,7 +9067,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -8651,7 +9075,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -8672,33 +9096,33 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -8757,7 +9181,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>177</v>
       </c>

</xml_diff>